<commit_message>
Matplotlib is inserted in the project by the author
</commit_message>
<xml_diff>
--- a/kayitlarx.xlsx
+++ b/kayitlarx.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:L6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -440,6 +440,33 @@
       <c r="C1" s="1" t="n">
         <v>1</v>
       </c>
+      <c r="D1" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="F1" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="G1" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="H1" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="I1" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="J1" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="K1" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="L1" s="1" t="n">
+        <v>10</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
@@ -453,6 +480,33 @@
       <c r="C2" t="n">
         <v>1</v>
       </c>
+      <c r="D2" t="n">
+        <v>2</v>
+      </c>
+      <c r="E2" t="n">
+        <v>3</v>
+      </c>
+      <c r="F2" t="n">
+        <v>4</v>
+      </c>
+      <c r="G2" t="n">
+        <v>5</v>
+      </c>
+      <c r="H2" t="n">
+        <v>6</v>
+      </c>
+      <c r="I2" t="n">
+        <v>9</v>
+      </c>
+      <c r="J2" t="n">
+        <v>9</v>
+      </c>
+      <c r="K2" t="n">
+        <v>12</v>
+      </c>
+      <c r="L2" t="n">
+        <v>12</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
@@ -464,7 +518,34 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>95.45999999999999</v>
+        <v>42.43</v>
+      </c>
+      <c r="D3" t="n">
+        <v>55.9</v>
+      </c>
+      <c r="E3" t="n">
+        <v>49.24</v>
+      </c>
+      <c r="F3" t="n">
+        <v>43.01</v>
+      </c>
+      <c r="G3" t="n">
+        <v>33.54</v>
+      </c>
+      <c r="H3" t="n">
+        <v>40.31</v>
+      </c>
+      <c r="I3" t="n">
+        <v>47.17</v>
+      </c>
+      <c r="J3" t="n">
+        <v>31.62</v>
+      </c>
+      <c r="K3" t="n">
+        <v>40.31</v>
+      </c>
+      <c r="L3" t="n">
+        <v>44.72</v>
       </c>
     </row>
     <row r="4">
@@ -477,7 +558,34 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>59.1</v>
+        <v>112.13</v>
+      </c>
+      <c r="D4" t="n">
+        <v>179.51</v>
+      </c>
+      <c r="E4" t="n">
+        <v>146.22</v>
+      </c>
+      <c r="F4" t="n">
+        <v>115.06</v>
+      </c>
+      <c r="G4" t="n">
+        <v>67.70999999999999</v>
+      </c>
+      <c r="H4" t="n">
+        <v>101.56</v>
+      </c>
+      <c r="I4" t="n">
+        <v>135.85</v>
+      </c>
+      <c r="J4" t="n">
+        <v>58.11</v>
+      </c>
+      <c r="K4" t="n">
+        <v>101.56</v>
+      </c>
+      <c r="L4" t="n">
+        <v>123.61</v>
       </c>
     </row>
     <row r="5">
@@ -492,6 +600,33 @@
       <c r="C5" t="n">
         <v>6440</v>
       </c>
+      <c r="D5" t="n">
+        <v>6440</v>
+      </c>
+      <c r="E5" t="n">
+        <v>6440</v>
+      </c>
+      <c r="F5" t="n">
+        <v>6440</v>
+      </c>
+      <c r="G5" t="n">
+        <v>6440</v>
+      </c>
+      <c r="H5" t="n">
+        <v>6440</v>
+      </c>
+      <c r="I5" t="n">
+        <v>6440</v>
+      </c>
+      <c r="J5" t="n">
+        <v>6440</v>
+      </c>
+      <c r="K5" t="n">
+        <v>6440</v>
+      </c>
+      <c r="L5" t="n">
+        <v>6440</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="n">
@@ -503,6 +638,33 @@
         </is>
       </c>
       <c r="C6" t="n">
+        <v>50</v>
+      </c>
+      <c r="D6" t="n">
+        <v>50</v>
+      </c>
+      <c r="E6" t="n">
+        <v>50</v>
+      </c>
+      <c r="F6" t="n">
+        <v>50</v>
+      </c>
+      <c r="G6" t="n">
+        <v>50</v>
+      </c>
+      <c r="H6" t="n">
+        <v>50</v>
+      </c>
+      <c r="I6" t="n">
+        <v>50</v>
+      </c>
+      <c r="J6" t="n">
+        <v>50</v>
+      </c>
+      <c r="K6" t="n">
+        <v>50</v>
+      </c>
+      <c r="L6" t="n">
         <v>50</v>
       </c>
     </row>

</xml_diff>

<commit_message>
pie charts are imported by the author
</commit_message>
<xml_diff>
--- a/kayitlarx.xlsx
+++ b/kayitlarx.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L6"/>
+  <dimension ref="A1:BM6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -467,6 +467,165 @@
       <c r="L1" s="1" t="n">
         <v>10</v>
       </c>
+      <c r="M1" s="1" t="n">
+        <v>11</v>
+      </c>
+      <c r="N1" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="O1" s="1" t="n">
+        <v>13</v>
+      </c>
+      <c r="P1" s="1" t="n">
+        <v>14</v>
+      </c>
+      <c r="Q1" s="1" t="n">
+        <v>15</v>
+      </c>
+      <c r="R1" s="1" t="n">
+        <v>16</v>
+      </c>
+      <c r="S1" s="1" t="n">
+        <v>17</v>
+      </c>
+      <c r="T1" s="1" t="n">
+        <v>18</v>
+      </c>
+      <c r="U1" s="1" t="n">
+        <v>19</v>
+      </c>
+      <c r="V1" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="W1" s="1" t="n">
+        <v>21</v>
+      </c>
+      <c r="X1" s="1" t="n">
+        <v>22</v>
+      </c>
+      <c r="Y1" s="1" t="n">
+        <v>23</v>
+      </c>
+      <c r="Z1" s="1" t="n">
+        <v>24</v>
+      </c>
+      <c r="AA1" s="1" t="n">
+        <v>25</v>
+      </c>
+      <c r="AB1" s="1" t="n">
+        <v>26</v>
+      </c>
+      <c r="AC1" s="1" t="n">
+        <v>27</v>
+      </c>
+      <c r="AD1" s="1" t="n">
+        <v>28</v>
+      </c>
+      <c r="AE1" s="1" t="n">
+        <v>29</v>
+      </c>
+      <c r="AF1" s="1" t="n">
+        <v>30</v>
+      </c>
+      <c r="AG1" s="1" t="n">
+        <v>31</v>
+      </c>
+      <c r="AH1" s="1" t="n">
+        <v>32</v>
+      </c>
+      <c r="AI1" s="1" t="n">
+        <v>33</v>
+      </c>
+      <c r="AJ1" s="1" t="n">
+        <v>34</v>
+      </c>
+      <c r="AK1" s="1" t="n">
+        <v>35</v>
+      </c>
+      <c r="AL1" s="1" t="n">
+        <v>36</v>
+      </c>
+      <c r="AM1" s="1" t="n">
+        <v>37</v>
+      </c>
+      <c r="AN1" s="1" t="n">
+        <v>38</v>
+      </c>
+      <c r="AO1" s="1" t="n">
+        <v>39</v>
+      </c>
+      <c r="AP1" s="1" t="n">
+        <v>40</v>
+      </c>
+      <c r="AQ1" s="1" t="n">
+        <v>41</v>
+      </c>
+      <c r="AR1" s="1" t="n">
+        <v>42</v>
+      </c>
+      <c r="AS1" s="1" t="n">
+        <v>43</v>
+      </c>
+      <c r="AT1" s="1" t="n">
+        <v>44</v>
+      </c>
+      <c r="AU1" s="1" t="n">
+        <v>45</v>
+      </c>
+      <c r="AV1" s="1" t="n">
+        <v>46</v>
+      </c>
+      <c r="AW1" s="1" t="n">
+        <v>47</v>
+      </c>
+      <c r="AX1" s="1" t="n">
+        <v>48</v>
+      </c>
+      <c r="AY1" s="1" t="n">
+        <v>49</v>
+      </c>
+      <c r="AZ1" s="1" t="n">
+        <v>50</v>
+      </c>
+      <c r="BA1" s="1" t="n">
+        <v>51</v>
+      </c>
+      <c r="BB1" s="1" t="n">
+        <v>52</v>
+      </c>
+      <c r="BC1" s="1" t="n">
+        <v>53</v>
+      </c>
+      <c r="BD1" s="1" t="n">
+        <v>54</v>
+      </c>
+      <c r="BE1" s="1" t="n">
+        <v>55</v>
+      </c>
+      <c r="BF1" s="1" t="n">
+        <v>56</v>
+      </c>
+      <c r="BG1" s="1" t="n">
+        <v>57</v>
+      </c>
+      <c r="BH1" s="1" t="n">
+        <v>58</v>
+      </c>
+      <c r="BI1" s="1" t="n">
+        <v>59</v>
+      </c>
+      <c r="BJ1" s="1" t="n">
+        <v>60</v>
+      </c>
+      <c r="BK1" s="1" t="n">
+        <v>61</v>
+      </c>
+      <c r="BL1" s="1" t="n">
+        <v>62</v>
+      </c>
+      <c r="BM1" s="1" t="n">
+        <v>63</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
@@ -478,34 +637,193 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="D2" t="n">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="E2" t="n">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="F2" t="n">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="G2" t="n">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="H2" t="n">
-        <v>6</v>
+        <v>19</v>
       </c>
       <c r="I2" t="n">
-        <v>9</v>
+        <v>20</v>
       </c>
       <c r="J2" t="n">
-        <v>9</v>
+        <v>24</v>
       </c>
       <c r="K2" t="n">
-        <v>12</v>
+        <v>25</v>
       </c>
       <c r="L2" t="n">
-        <v>12</v>
+        <v>28</v>
+      </c>
+      <c r="M2" t="n">
+        <v>30</v>
+      </c>
+      <c r="N2" t="n">
+        <v>35</v>
+      </c>
+      <c r="O2" t="n">
+        <v>36</v>
+      </c>
+      <c r="P2" t="n">
+        <v>38</v>
+      </c>
+      <c r="Q2" t="n">
+        <v>40</v>
+      </c>
+      <c r="R2" t="n">
+        <v>43</v>
+      </c>
+      <c r="S2" t="n">
+        <v>43</v>
+      </c>
+      <c r="T2" t="n">
+        <v>43</v>
+      </c>
+      <c r="U2" t="n">
+        <v>44</v>
+      </c>
+      <c r="V2" t="n">
+        <v>45</v>
+      </c>
+      <c r="W2" t="n">
+        <v>46</v>
+      </c>
+      <c r="X2" t="n">
+        <v>47</v>
+      </c>
+      <c r="Y2" t="n">
+        <v>51</v>
+      </c>
+      <c r="Z2" t="n">
+        <v>53</v>
+      </c>
+      <c r="AA2" t="n">
+        <v>55</v>
+      </c>
+      <c r="AB2" t="n">
+        <v>56</v>
+      </c>
+      <c r="AC2" t="n">
+        <v>57</v>
+      </c>
+      <c r="AD2" t="n">
+        <v>60</v>
+      </c>
+      <c r="AE2" t="n">
+        <v>63</v>
+      </c>
+      <c r="AF2" t="n">
+        <v>64</v>
+      </c>
+      <c r="AG2" t="n">
+        <v>66</v>
+      </c>
+      <c r="AH2" t="n">
+        <v>66</v>
+      </c>
+      <c r="AI2" t="n">
+        <v>70</v>
+      </c>
+      <c r="AJ2" t="n">
+        <v>71</v>
+      </c>
+      <c r="AK2" t="n">
+        <v>72</v>
+      </c>
+      <c r="AL2" t="n">
+        <v>78</v>
+      </c>
+      <c r="AM2" t="n">
+        <v>79</v>
+      </c>
+      <c r="AN2" t="n">
+        <v>83</v>
+      </c>
+      <c r="AO2" t="n">
+        <v>91</v>
+      </c>
+      <c r="AP2" t="n">
+        <v>96</v>
+      </c>
+      <c r="AQ2" t="n">
+        <v>97</v>
+      </c>
+      <c r="AR2" t="n">
+        <v>101</v>
+      </c>
+      <c r="AS2" t="n">
+        <v>102</v>
+      </c>
+      <c r="AT2" t="n">
+        <v>105</v>
+      </c>
+      <c r="AU2" t="n">
+        <v>106</v>
+      </c>
+      <c r="AV2" t="n">
+        <v>108</v>
+      </c>
+      <c r="AW2" t="n">
+        <v>109</v>
+      </c>
+      <c r="AX2" t="n">
+        <v>115</v>
+      </c>
+      <c r="AY2" t="n">
+        <v>119</v>
+      </c>
+      <c r="AZ2" t="n">
+        <v>122</v>
+      </c>
+      <c r="BA2" t="n">
+        <v>123</v>
+      </c>
+      <c r="BB2" t="n">
+        <v>125</v>
+      </c>
+      <c r="BC2" t="n">
+        <v>132</v>
+      </c>
+      <c r="BD2" t="n">
+        <v>133</v>
+      </c>
+      <c r="BE2" t="n">
+        <v>135</v>
+      </c>
+      <c r="BF2" t="n">
+        <v>135</v>
+      </c>
+      <c r="BG2" t="n">
+        <v>141</v>
+      </c>
+      <c r="BH2" t="n">
+        <v>141</v>
+      </c>
+      <c r="BI2" t="n">
+        <v>149</v>
+      </c>
+      <c r="BJ2" t="n">
+        <v>149</v>
+      </c>
+      <c r="BK2" t="n">
+        <v>150</v>
+      </c>
+      <c r="BL2" t="n">
+        <v>152</v>
+      </c>
+      <c r="BM2" t="n">
+        <v>155</v>
       </c>
     </row>
     <row r="3">
@@ -518,34 +836,193 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>42.43</v>
+        <v>61.85</v>
       </c>
       <c r="D3" t="n">
         <v>55.9</v>
       </c>
       <c r="E3" t="n">
-        <v>49.24</v>
+        <v>110.11</v>
       </c>
       <c r="F3" t="n">
-        <v>43.01</v>
+        <v>101.24</v>
       </c>
       <c r="G3" t="n">
-        <v>33.54</v>
+        <v>58.31</v>
       </c>
       <c r="H3" t="n">
-        <v>40.31</v>
+        <v>78.09999999999999</v>
       </c>
       <c r="I3" t="n">
-        <v>47.17</v>
+        <v>71.06</v>
       </c>
       <c r="J3" t="n">
-        <v>31.62</v>
+        <v>58.31</v>
       </c>
       <c r="K3" t="n">
-        <v>40.31</v>
+        <v>57.01</v>
       </c>
       <c r="L3" t="n">
-        <v>44.72</v>
+        <v>80.62</v>
+      </c>
+      <c r="M3" t="n">
+        <v>75</v>
+      </c>
+      <c r="N3" t="n">
+        <v>69.64</v>
+      </c>
+      <c r="O3" t="n">
+        <v>80.62</v>
+      </c>
+      <c r="P3" t="n">
+        <v>79.06</v>
+      </c>
+      <c r="Q3" t="n">
+        <v>73.81999999999999</v>
+      </c>
+      <c r="R3" t="n">
+        <v>63.64</v>
+      </c>
+      <c r="S3" t="n">
+        <v>55.9</v>
+      </c>
+      <c r="T3" t="n">
+        <v>55.9</v>
+      </c>
+      <c r="U3" t="n">
+        <v>87.45999999999999</v>
+      </c>
+      <c r="V3" t="n">
+        <v>69.45999999999999</v>
+      </c>
+      <c r="W3" t="n">
+        <v>55.9</v>
+      </c>
+      <c r="X3" t="n">
+        <v>64.03</v>
+      </c>
+      <c r="Y3" t="n">
+        <v>78.26000000000001</v>
+      </c>
+      <c r="Z3" t="n">
+        <v>70.70999999999999</v>
+      </c>
+      <c r="AA3" t="n">
+        <v>60.83</v>
+      </c>
+      <c r="AB3" t="n">
+        <v>57.01</v>
+      </c>
+      <c r="AC3" t="n">
+        <v>61.85</v>
+      </c>
+      <c r="AD3" t="n">
+        <v>83.22</v>
+      </c>
+      <c r="AE3" t="n">
+        <v>63.25</v>
+      </c>
+      <c r="AF3" t="n">
+        <v>58.31</v>
+      </c>
+      <c r="AG3" t="n">
+        <v>112.36</v>
+      </c>
+      <c r="AH3" t="n">
+        <v>62.65</v>
+      </c>
+      <c r="AI3" t="n">
+        <v>62.65</v>
+      </c>
+      <c r="AJ3" t="n">
+        <v>71.06</v>
+      </c>
+      <c r="AK3" t="n">
+        <v>65.19</v>
+      </c>
+      <c r="AL3" t="n">
+        <v>62.65</v>
+      </c>
+      <c r="AM3" t="n">
+        <v>80.62</v>
+      </c>
+      <c r="AN3" t="n">
+        <v>63.25</v>
+      </c>
+      <c r="AO3" t="n">
+        <v>66.70999999999999</v>
+      </c>
+      <c r="AP3" t="n">
+        <v>65.19</v>
+      </c>
+      <c r="AQ3" t="n">
+        <v>55.23</v>
+      </c>
+      <c r="AR3" t="n">
+        <v>67.27</v>
+      </c>
+      <c r="AS3" t="n">
+        <v>67.27</v>
+      </c>
+      <c r="AT3" t="n">
+        <v>70.70999999999999</v>
+      </c>
+      <c r="AU3" t="n">
+        <v>83.22</v>
+      </c>
+      <c r="AV3" t="n">
+        <v>70.18000000000001</v>
+      </c>
+      <c r="AW3" t="n">
+        <v>70.70999999999999</v>
+      </c>
+      <c r="AX3" t="n">
+        <v>80.62</v>
+      </c>
+      <c r="AY3" t="n">
+        <v>69.64</v>
+      </c>
+      <c r="AZ3" t="n">
+        <v>61.85</v>
+      </c>
+      <c r="BA3" t="n">
+        <v>76.31999999999999</v>
+      </c>
+      <c r="BB3" t="n">
+        <v>55.9</v>
+      </c>
+      <c r="BC3" t="n">
+        <v>69.45999999999999</v>
+      </c>
+      <c r="BD3" t="n">
+        <v>60.21</v>
+      </c>
+      <c r="BE3" t="n">
+        <v>57.01</v>
+      </c>
+      <c r="BF3" t="n">
+        <v>65.19</v>
+      </c>
+      <c r="BG3" t="n">
+        <v>74.33</v>
+      </c>
+      <c r="BH3" t="n">
+        <v>60.42</v>
+      </c>
+      <c r="BI3" t="n">
+        <v>58.31</v>
+      </c>
+      <c r="BJ3" t="n">
+        <v>55.9</v>
+      </c>
+      <c r="BK3" t="n">
+        <v>57.01</v>
+      </c>
+      <c r="BL3" t="n">
+        <v>65.19</v>
+      </c>
+      <c r="BM3" t="n">
+        <v>77.62</v>
       </c>
     </row>
     <row r="4">
@@ -558,34 +1035,193 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>112.13</v>
+        <v>23.69</v>
       </c>
       <c r="D4" t="n">
-        <v>179.51</v>
+        <v>11.8</v>
       </c>
       <c r="E4" t="n">
-        <v>146.22</v>
+        <v>120.23</v>
       </c>
       <c r="F4" t="n">
-        <v>115.06</v>
+        <v>102.48</v>
       </c>
       <c r="G4" t="n">
-        <v>67.70999999999999</v>
+        <v>16.62</v>
       </c>
       <c r="H4" t="n">
-        <v>101.56</v>
+        <v>56.2</v>
       </c>
       <c r="I4" t="n">
-        <v>135.85</v>
+        <v>42.13</v>
       </c>
       <c r="J4" t="n">
+        <v>16.62</v>
+      </c>
+      <c r="K4" t="n">
+        <v>14.02</v>
+      </c>
+      <c r="L4" t="n">
+        <v>61.25</v>
+      </c>
+      <c r="M4" t="n">
+        <v>50</v>
+      </c>
+      <c r="N4" t="n">
+        <v>39.28</v>
+      </c>
+      <c r="O4" t="n">
+        <v>61.25</v>
+      </c>
+      <c r="P4" t="n">
         <v>58.11</v>
       </c>
-      <c r="K4" t="n">
-        <v>101.56</v>
-      </c>
-      <c r="L4" t="n">
-        <v>123.61</v>
+      <c r="Q4" t="n">
+        <v>47.65</v>
+      </c>
+      <c r="R4" t="n">
+        <v>27.28</v>
+      </c>
+      <c r="S4" t="n">
+        <v>11.8</v>
+      </c>
+      <c r="T4" t="n">
+        <v>11.8</v>
+      </c>
+      <c r="U4" t="n">
+        <v>74.93000000000001</v>
+      </c>
+      <c r="V4" t="n">
+        <v>38.92</v>
+      </c>
+      <c r="W4" t="n">
+        <v>11.8</v>
+      </c>
+      <c r="X4" t="n">
+        <v>28.06</v>
+      </c>
+      <c r="Y4" t="n">
+        <v>56.52</v>
+      </c>
+      <c r="Z4" t="n">
+        <v>41.42</v>
+      </c>
+      <c r="AA4" t="n">
+        <v>21.66</v>
+      </c>
+      <c r="AB4" t="n">
+        <v>14.02</v>
+      </c>
+      <c r="AC4" t="n">
+        <v>23.69</v>
+      </c>
+      <c r="AD4" t="n">
+        <v>66.43000000000001</v>
+      </c>
+      <c r="AE4" t="n">
+        <v>26.49</v>
+      </c>
+      <c r="AF4" t="n">
+        <v>16.62</v>
+      </c>
+      <c r="AG4" t="n">
+        <v>124.72</v>
+      </c>
+      <c r="AH4" t="n">
+        <v>25.3</v>
+      </c>
+      <c r="AI4" t="n">
+        <v>25.3</v>
+      </c>
+      <c r="AJ4" t="n">
+        <v>42.13</v>
+      </c>
+      <c r="AK4" t="n">
+        <v>30.38</v>
+      </c>
+      <c r="AL4" t="n">
+        <v>25.3</v>
+      </c>
+      <c r="AM4" t="n">
+        <v>61.25</v>
+      </c>
+      <c r="AN4" t="n">
+        <v>26.49</v>
+      </c>
+      <c r="AO4" t="n">
+        <v>33.42</v>
+      </c>
+      <c r="AP4" t="n">
+        <v>30.38</v>
+      </c>
+      <c r="AQ4" t="n">
+        <v>10.45</v>
+      </c>
+      <c r="AR4" t="n">
+        <v>34.54</v>
+      </c>
+      <c r="AS4" t="n">
+        <v>34.54</v>
+      </c>
+      <c r="AT4" t="n">
+        <v>41.42</v>
+      </c>
+      <c r="AU4" t="n">
+        <v>66.43000000000001</v>
+      </c>
+      <c r="AV4" t="n">
+        <v>40.36</v>
+      </c>
+      <c r="AW4" t="n">
+        <v>41.42</v>
+      </c>
+      <c r="AX4" t="n">
+        <v>61.25</v>
+      </c>
+      <c r="AY4" t="n">
+        <v>39.28</v>
+      </c>
+      <c r="AZ4" t="n">
+        <v>23.69</v>
+      </c>
+      <c r="BA4" t="n">
+        <v>52.64</v>
+      </c>
+      <c r="BB4" t="n">
+        <v>11.8</v>
+      </c>
+      <c r="BC4" t="n">
+        <v>38.92</v>
+      </c>
+      <c r="BD4" t="n">
+        <v>20.42</v>
+      </c>
+      <c r="BE4" t="n">
+        <v>14.02</v>
+      </c>
+      <c r="BF4" t="n">
+        <v>30.38</v>
+      </c>
+      <c r="BG4" t="n">
+        <v>48.66</v>
+      </c>
+      <c r="BH4" t="n">
+        <v>20.83</v>
+      </c>
+      <c r="BI4" t="n">
+        <v>16.62</v>
+      </c>
+      <c r="BJ4" t="n">
+        <v>11.8</v>
+      </c>
+      <c r="BK4" t="n">
+        <v>14.02</v>
+      </c>
+      <c r="BL4" t="n">
+        <v>30.38</v>
+      </c>
+      <c r="BM4" t="n">
+        <v>55.24</v>
       </c>
     </row>
     <row r="5">
@@ -598,10 +1234,10 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>6440</v>
+        <v>1508.5</v>
       </c>
       <c r="D5" t="n">
-        <v>6440</v>
+        <v>1508.5</v>
       </c>
       <c r="E5" t="n">
         <v>6440</v>
@@ -610,21 +1246,180 @@
         <v>6440</v>
       </c>
       <c r="G5" t="n">
-        <v>6440</v>
+        <v>1508.5</v>
       </c>
       <c r="H5" t="n">
         <v>6440</v>
       </c>
       <c r="I5" t="n">
+        <v>3136</v>
+      </c>
+      <c r="J5" t="n">
+        <v>1508.5</v>
+      </c>
+      <c r="K5" t="n">
+        <v>1508.5</v>
+      </c>
+      <c r="L5" t="n">
         <v>6440</v>
       </c>
-      <c r="J5" t="n">
+      <c r="M5" t="n">
         <v>6440</v>
       </c>
-      <c r="K5" t="n">
+      <c r="N5" t="n">
+        <v>3136</v>
+      </c>
+      <c r="O5" t="n">
         <v>6440</v>
       </c>
-      <c r="L5" t="n">
+      <c r="P5" t="n">
+        <v>6440</v>
+      </c>
+      <c r="Q5" t="n">
+        <v>3136</v>
+      </c>
+      <c r="R5" t="n">
+        <v>1508.5</v>
+      </c>
+      <c r="S5" t="n">
+        <v>1508.5</v>
+      </c>
+      <c r="T5" t="n">
+        <v>1508.5</v>
+      </c>
+      <c r="U5" t="n">
+        <v>6440</v>
+      </c>
+      <c r="V5" t="n">
+        <v>3136</v>
+      </c>
+      <c r="W5" t="n">
+        <v>1508.5</v>
+      </c>
+      <c r="X5" t="n">
+        <v>1508.5</v>
+      </c>
+      <c r="Y5" t="n">
+        <v>6440</v>
+      </c>
+      <c r="Z5" t="n">
+        <v>3136</v>
+      </c>
+      <c r="AA5" t="n">
+        <v>1508.5</v>
+      </c>
+      <c r="AB5" t="n">
+        <v>1508.5</v>
+      </c>
+      <c r="AC5" t="n">
+        <v>1508.5</v>
+      </c>
+      <c r="AD5" t="n">
+        <v>6440</v>
+      </c>
+      <c r="AE5" t="n">
+        <v>1508.5</v>
+      </c>
+      <c r="AF5" t="n">
+        <v>1508.5</v>
+      </c>
+      <c r="AG5" t="n">
+        <v>6440</v>
+      </c>
+      <c r="AH5" t="n">
+        <v>1508.5</v>
+      </c>
+      <c r="AI5" t="n">
+        <v>1508.5</v>
+      </c>
+      <c r="AJ5" t="n">
+        <v>3136</v>
+      </c>
+      <c r="AK5" t="n">
+        <v>3136</v>
+      </c>
+      <c r="AL5" t="n">
+        <v>1508.5</v>
+      </c>
+      <c r="AM5" t="n">
+        <v>6440</v>
+      </c>
+      <c r="AN5" t="n">
+        <v>1508.5</v>
+      </c>
+      <c r="AO5" t="n">
+        <v>3136</v>
+      </c>
+      <c r="AP5" t="n">
+        <v>3136</v>
+      </c>
+      <c r="AQ5" t="n">
+        <v>1508.5</v>
+      </c>
+      <c r="AR5" t="n">
+        <v>3136</v>
+      </c>
+      <c r="AS5" t="n">
+        <v>3136</v>
+      </c>
+      <c r="AT5" t="n">
+        <v>3136</v>
+      </c>
+      <c r="AU5" t="n">
+        <v>6440</v>
+      </c>
+      <c r="AV5" t="n">
+        <v>3136</v>
+      </c>
+      <c r="AW5" t="n">
+        <v>3136</v>
+      </c>
+      <c r="AX5" t="n">
+        <v>6440</v>
+      </c>
+      <c r="AY5" t="n">
+        <v>3136</v>
+      </c>
+      <c r="AZ5" t="n">
+        <v>1508.5</v>
+      </c>
+      <c r="BA5" t="n">
+        <v>6440</v>
+      </c>
+      <c r="BB5" t="n">
+        <v>1508.5</v>
+      </c>
+      <c r="BC5" t="n">
+        <v>3136</v>
+      </c>
+      <c r="BD5" t="n">
+        <v>1508.5</v>
+      </c>
+      <c r="BE5" t="n">
+        <v>1508.5</v>
+      </c>
+      <c r="BF5" t="n">
+        <v>3136</v>
+      </c>
+      <c r="BG5" t="n">
+        <v>3136</v>
+      </c>
+      <c r="BH5" t="n">
+        <v>1508.5</v>
+      </c>
+      <c r="BI5" t="n">
+        <v>1508.5</v>
+      </c>
+      <c r="BJ5" t="n">
+        <v>1508.5</v>
+      </c>
+      <c r="BK5" t="n">
+        <v>1508.5</v>
+      </c>
+      <c r="BL5" t="n">
+        <v>3136</v>
+      </c>
+      <c r="BM5" t="n">
         <v>6440</v>
       </c>
     </row>
@@ -638,10 +1433,10 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>50</v>
+        <v>10</v>
       </c>
       <c r="D6" t="n">
-        <v>50</v>
+        <v>10</v>
       </c>
       <c r="E6" t="n">
         <v>50</v>
@@ -650,21 +1445,180 @@
         <v>50</v>
       </c>
       <c r="G6" t="n">
-        <v>50</v>
+        <v>10</v>
       </c>
       <c r="H6" t="n">
         <v>50</v>
       </c>
       <c r="I6" t="n">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="J6" t="n">
-        <v>50</v>
+        <v>10</v>
       </c>
       <c r="K6" t="n">
-        <v>50</v>
+        <v>10</v>
       </c>
       <c r="L6" t="n">
+        <v>50</v>
+      </c>
+      <c r="M6" t="n">
+        <v>50</v>
+      </c>
+      <c r="N6" t="n">
+        <v>30</v>
+      </c>
+      <c r="O6" t="n">
+        <v>50</v>
+      </c>
+      <c r="P6" t="n">
+        <v>50</v>
+      </c>
+      <c r="Q6" t="n">
+        <v>30</v>
+      </c>
+      <c r="R6" t="n">
+        <v>10</v>
+      </c>
+      <c r="S6" t="n">
+        <v>10</v>
+      </c>
+      <c r="T6" t="n">
+        <v>10</v>
+      </c>
+      <c r="U6" t="n">
+        <v>50</v>
+      </c>
+      <c r="V6" t="n">
+        <v>30</v>
+      </c>
+      <c r="W6" t="n">
+        <v>10</v>
+      </c>
+      <c r="X6" t="n">
+        <v>10</v>
+      </c>
+      <c r="Y6" t="n">
+        <v>50</v>
+      </c>
+      <c r="Z6" t="n">
+        <v>30</v>
+      </c>
+      <c r="AA6" t="n">
+        <v>10</v>
+      </c>
+      <c r="AB6" t="n">
+        <v>10</v>
+      </c>
+      <c r="AC6" t="n">
+        <v>10</v>
+      </c>
+      <c r="AD6" t="n">
+        <v>50</v>
+      </c>
+      <c r="AE6" t="n">
+        <v>10</v>
+      </c>
+      <c r="AF6" t="n">
+        <v>10</v>
+      </c>
+      <c r="AG6" t="n">
+        <v>50</v>
+      </c>
+      <c r="AH6" t="n">
+        <v>10</v>
+      </c>
+      <c r="AI6" t="n">
+        <v>10</v>
+      </c>
+      <c r="AJ6" t="n">
+        <v>30</v>
+      </c>
+      <c r="AK6" t="n">
+        <v>30</v>
+      </c>
+      <c r="AL6" t="n">
+        <v>10</v>
+      </c>
+      <c r="AM6" t="n">
+        <v>50</v>
+      </c>
+      <c r="AN6" t="n">
+        <v>10</v>
+      </c>
+      <c r="AO6" t="n">
+        <v>30</v>
+      </c>
+      <c r="AP6" t="n">
+        <v>30</v>
+      </c>
+      <c r="AQ6" t="n">
+        <v>10</v>
+      </c>
+      <c r="AR6" t="n">
+        <v>30</v>
+      </c>
+      <c r="AS6" t="n">
+        <v>30</v>
+      </c>
+      <c r="AT6" t="n">
+        <v>30</v>
+      </c>
+      <c r="AU6" t="n">
+        <v>50</v>
+      </c>
+      <c r="AV6" t="n">
+        <v>30</v>
+      </c>
+      <c r="AW6" t="n">
+        <v>30</v>
+      </c>
+      <c r="AX6" t="n">
+        <v>50</v>
+      </c>
+      <c r="AY6" t="n">
+        <v>30</v>
+      </c>
+      <c r="AZ6" t="n">
+        <v>10</v>
+      </c>
+      <c r="BA6" t="n">
+        <v>50</v>
+      </c>
+      <c r="BB6" t="n">
+        <v>10</v>
+      </c>
+      <c r="BC6" t="n">
+        <v>30</v>
+      </c>
+      <c r="BD6" t="n">
+        <v>10</v>
+      </c>
+      <c r="BE6" t="n">
+        <v>10</v>
+      </c>
+      <c r="BF6" t="n">
+        <v>30</v>
+      </c>
+      <c r="BG6" t="n">
+        <v>30</v>
+      </c>
+      <c r="BH6" t="n">
+        <v>10</v>
+      </c>
+      <c r="BI6" t="n">
+        <v>10</v>
+      </c>
+      <c r="BJ6" t="n">
+        <v>10</v>
+      </c>
+      <c r="BK6" t="n">
+        <v>10</v>
+      </c>
+      <c r="BL6" t="n">
+        <v>30</v>
+      </c>
+      <c r="BM6" t="n">
         <v>50</v>
       </c>
     </row>

</xml_diff>

<commit_message>
the property of taking screenshot is imported
</commit_message>
<xml_diff>
--- a/kayitlarx.xlsx
+++ b/kayitlarx.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J6"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -435,200 +435,58 @@
   <sheetData>
     <row r="1">
       <c r="B1" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="C1" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="D1" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="E1" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="F1" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="G1" s="1" t="n">
-        <v>5</v>
-      </c>
-      <c r="H1" s="1" t="n">
-        <v>6</v>
-      </c>
-      <c r="I1" s="1" t="n">
-        <v>7</v>
-      </c>
-      <c r="J1" s="1" t="n">
-        <v>8</v>
-      </c>
     </row>
     <row r="2">
-      <c r="A2" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="B2" t="inlineStr">
+      <c r="A2" s="1" t="inlineStr">
         <is>
           <t>carID</t>
         </is>
       </c>
-      <c r="C2" t="n">
+      <c r="B2" t="n">
         <v>1</v>
       </c>
-      <c r="D2" t="n">
-        <v>2</v>
-      </c>
-      <c r="E2" t="n">
-        <v>3</v>
-      </c>
-      <c r="F2" t="n">
-        <v>4</v>
-      </c>
-      <c r="G2" t="n">
-        <v>6</v>
-      </c>
-      <c r="H2" t="n">
-        <v>9</v>
-      </c>
-      <c r="I2" t="n">
-        <v>12</v>
-      </c>
-      <c r="J2" t="n">
-        <v>12</v>
-      </c>
     </row>
     <row r="3">
-      <c r="A3" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="B3" t="inlineStr">
+      <c r="A3" s="1" t="inlineStr">
         <is>
           <t>speed2</t>
         </is>
       </c>
-      <c r="C3" t="n">
+      <c r="B3" t="n">
         <v>42.43</v>
       </c>
-      <c r="D3" t="n">
-        <v>55.9</v>
-      </c>
-      <c r="E3" t="n">
-        <v>49.24</v>
-      </c>
-      <c r="F3" t="n">
-        <v>43.01</v>
-      </c>
-      <c r="G3" t="n">
-        <v>40.31</v>
-      </c>
-      <c r="H3" t="n">
-        <v>47.17</v>
-      </c>
-      <c r="I3" t="n">
-        <v>40.31</v>
-      </c>
-      <c r="J3" t="n">
-        <v>44.72</v>
-      </c>
     </row>
     <row r="4">
-      <c r="A4" s="1" t="n">
-        <v>2</v>
+      <c r="A4" s="1" t="inlineStr">
+        <is>
+          <t>asma</t>
+        </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>asma</t>
-        </is>
-      </c>
-      <c r="C4" t="n">
-        <v>21.22</v>
-      </c>
-      <c r="D4" t="n">
-        <v>59.72</v>
-      </c>
-      <c r="E4" t="n">
-        <v>40.7</v>
-      </c>
-      <c r="F4" t="n">
-        <v>22.89</v>
-      </c>
-      <c r="G4" t="n">
-        <v>15.18</v>
-      </c>
-      <c r="H4" t="n">
-        <v>34.77</v>
-      </c>
-      <c r="I4" t="n">
-        <v>15.18</v>
-      </c>
-      <c r="J4" t="n">
-        <v>27.78</v>
+          <t>21.22</t>
+        </is>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="B5" t="inlineStr">
+      <c r="A5" s="1" t="inlineStr">
         <is>
           <t>ceza_tutar</t>
         </is>
       </c>
-      <c r="C5" t="n">
+      <c r="B5" t="n">
         <v>1508.5</v>
       </c>
-      <c r="D5" t="n">
-        <v>6440</v>
-      </c>
-      <c r="E5" t="n">
-        <v>3136</v>
-      </c>
-      <c r="F5" t="n">
-        <v>1508.5</v>
-      </c>
-      <c r="G5" t="n">
-        <v>1508.5</v>
-      </c>
-      <c r="H5" t="n">
-        <v>3136</v>
-      </c>
-      <c r="I5" t="n">
-        <v>1508.5</v>
-      </c>
-      <c r="J5" t="n">
-        <v>1508.5</v>
-      </c>
     </row>
     <row r="6">
-      <c r="A6" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="B6" t="inlineStr">
+      <c r="A6" s="1" t="inlineStr">
         <is>
           <t>hesaplanan_asma</t>
         </is>
       </c>
-      <c r="C6" t="n">
-        <v>10</v>
-      </c>
-      <c r="D6" t="n">
-        <v>50</v>
-      </c>
-      <c r="E6" t="n">
-        <v>30</v>
-      </c>
-      <c r="F6" t="n">
-        <v>10</v>
-      </c>
-      <c r="G6" t="n">
-        <v>10</v>
-      </c>
-      <c r="H6" t="n">
-        <v>30</v>
-      </c>
-      <c r="I6" t="n">
-        <v>10</v>
-      </c>
-      <c r="J6" t="n">
+      <c r="B6" t="n">
         <v>10</v>
       </c>
     </row>

</xml_diff>

<commit_message>
screenshots are imported to the mail function as well
</commit_message>
<xml_diff>
--- a/kayitlarx.xlsx
+++ b/kayitlarx.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:J6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -435,58 +435,200 @@
   <sheetData>
     <row r="1">
       <c r="B1" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="n">
         <v>1</v>
+      </c>
+      <c r="D1" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="F1" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="G1" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="H1" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="I1" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="J1" s="1" t="n">
+        <v>8</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="1" t="inlineStr">
+      <c r="A2" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B2" t="inlineStr">
         <is>
           <t>carID</t>
         </is>
       </c>
-      <c r="B2" t="n">
+      <c r="C2" t="n">
         <v>1</v>
+      </c>
+      <c r="D2" t="n">
+        <v>2</v>
+      </c>
+      <c r="E2" t="n">
+        <v>3</v>
+      </c>
+      <c r="F2" t="n">
+        <v>4</v>
+      </c>
+      <c r="G2" t="n">
+        <v>6</v>
+      </c>
+      <c r="H2" t="n">
+        <v>9</v>
+      </c>
+      <c r="I2" t="n">
+        <v>12</v>
+      </c>
+      <c r="J2" t="n">
+        <v>12</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="1" t="inlineStr">
+      <c r="A3" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" t="inlineStr">
         <is>
           <t>speed2</t>
         </is>
       </c>
-      <c r="B3" t="n">
+      <c r="C3" t="n">
         <v>42.43</v>
+      </c>
+      <c r="D3" t="n">
+        <v>55.9</v>
+      </c>
+      <c r="E3" t="n">
+        <v>49.24</v>
+      </c>
+      <c r="F3" t="n">
+        <v>43.01</v>
+      </c>
+      <c r="G3" t="n">
+        <v>40.31</v>
+      </c>
+      <c r="H3" t="n">
+        <v>47.17</v>
+      </c>
+      <c r="I3" t="n">
+        <v>40.31</v>
+      </c>
+      <c r="J3" t="n">
+        <v>44.72</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="1" t="inlineStr">
+      <c r="A4" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="B4" t="inlineStr">
         <is>
           <t>asma</t>
         </is>
       </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>21.22</t>
-        </is>
+      <c r="C4" t="n">
+        <v>21.22</v>
+      </c>
+      <c r="D4" t="n">
+        <v>59.72</v>
+      </c>
+      <c r="E4" t="n">
+        <v>40.7</v>
+      </c>
+      <c r="F4" t="n">
+        <v>22.89</v>
+      </c>
+      <c r="G4" t="n">
+        <v>15.18</v>
+      </c>
+      <c r="H4" t="n">
+        <v>34.77</v>
+      </c>
+      <c r="I4" t="n">
+        <v>15.18</v>
+      </c>
+      <c r="J4" t="n">
+        <v>27.78</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="1" t="inlineStr">
+      <c r="A5" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="B5" t="inlineStr">
         <is>
           <t>ceza_tutar</t>
         </is>
       </c>
-      <c r="B5" t="n">
+      <c r="C5" t="n">
+        <v>1508.5</v>
+      </c>
+      <c r="D5" t="n">
+        <v>6440</v>
+      </c>
+      <c r="E5" t="n">
+        <v>3136</v>
+      </c>
+      <c r="F5" t="n">
+        <v>1508.5</v>
+      </c>
+      <c r="G5" t="n">
+        <v>1508.5</v>
+      </c>
+      <c r="H5" t="n">
+        <v>3136</v>
+      </c>
+      <c r="I5" t="n">
+        <v>1508.5</v>
+      </c>
+      <c r="J5" t="n">
         <v>1508.5</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="1" t="inlineStr">
+      <c r="A6" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="B6" t="inlineStr">
         <is>
           <t>hesaplanan_asma</t>
         </is>
       </c>
-      <c r="B6" t="n">
+      <c r="C6" t="n">
+        <v>10</v>
+      </c>
+      <c r="D6" t="n">
+        <v>50</v>
+      </c>
+      <c r="E6" t="n">
+        <v>30</v>
+      </c>
+      <c r="F6" t="n">
+        <v>10</v>
+      </c>
+      <c r="G6" t="n">
+        <v>10</v>
+      </c>
+      <c r="H6" t="n">
+        <v>30</v>
+      </c>
+      <c r="I6" t="n">
+        <v>10</v>
+      </c>
+      <c r="J6" t="n">
         <v>10</v>
       </c>
     </row>

</xml_diff>

<commit_message>
The file responsible for cropping the screenshots is imported.
</commit_message>
<xml_diff>
--- a/kayitlarx.xlsx
+++ b/kayitlarx.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J6"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -435,201 +435,79 @@
   <sheetData>
     <row r="1">
       <c r="B1" s="1" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C1" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="D1" s="1" t="n">
         <v>2</v>
-      </c>
-      <c r="E1" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="F1" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="G1" s="1" t="n">
-        <v>5</v>
-      </c>
-      <c r="H1" s="1" t="n">
-        <v>6</v>
-      </c>
-      <c r="I1" s="1" t="n">
-        <v>7</v>
-      </c>
-      <c r="J1" s="1" t="n">
-        <v>8</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="B2" t="inlineStr">
+      <c r="A2" s="1" t="inlineStr">
         <is>
           <t>carID</t>
         </is>
       </c>
+      <c r="B2" t="n">
+        <v>1</v>
+      </c>
       <c r="C2" t="n">
-        <v>1</v>
-      </c>
-      <c r="D2" t="n">
         <v>2</v>
-      </c>
-      <c r="E2" t="n">
-        <v>3</v>
-      </c>
-      <c r="F2" t="n">
-        <v>4</v>
-      </c>
-      <c r="G2" t="n">
-        <v>6</v>
-      </c>
-      <c r="H2" t="n">
-        <v>9</v>
-      </c>
-      <c r="I2" t="n">
-        <v>12</v>
-      </c>
-      <c r="J2" t="n">
-        <v>12</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="B3" t="inlineStr">
+      <c r="A3" s="1" t="inlineStr">
         <is>
           <t>speed2</t>
         </is>
       </c>
+      <c r="B3" t="n">
+        <v>42.43</v>
+      </c>
       <c r="C3" t="n">
-        <v>42.43</v>
-      </c>
-      <c r="D3" t="n">
         <v>55.9</v>
-      </c>
-      <c r="E3" t="n">
-        <v>49.24</v>
-      </c>
-      <c r="F3" t="n">
-        <v>43.01</v>
-      </c>
-      <c r="G3" t="n">
-        <v>40.31</v>
-      </c>
-      <c r="H3" t="n">
-        <v>47.17</v>
-      </c>
-      <c r="I3" t="n">
-        <v>40.31</v>
-      </c>
-      <c r="J3" t="n">
-        <v>44.72</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="1" t="n">
-        <v>2</v>
+      <c r="A4" s="1" t="inlineStr">
+        <is>
+          <t>asma</t>
+        </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>asma</t>
-        </is>
-      </c>
-      <c r="C4" t="n">
-        <v>21.22</v>
-      </c>
-      <c r="D4" t="n">
-        <v>59.72</v>
-      </c>
-      <c r="E4" t="n">
-        <v>40.7</v>
-      </c>
-      <c r="F4" t="n">
-        <v>22.89</v>
-      </c>
-      <c r="G4" t="n">
-        <v>15.18</v>
-      </c>
-      <c r="H4" t="n">
-        <v>34.77</v>
-      </c>
-      <c r="I4" t="n">
-        <v>15.18</v>
-      </c>
-      <c r="J4" t="n">
-        <v>27.78</v>
+          <t>21.22</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>59.72</t>
+        </is>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="B5" t="inlineStr">
+      <c r="A5" s="1" t="inlineStr">
         <is>
           <t>ceza_tutar</t>
         </is>
       </c>
+      <c r="B5" t="n">
+        <v>1508.5</v>
+      </c>
       <c r="C5" t="n">
-        <v>1508.5</v>
-      </c>
-      <c r="D5" t="n">
         <v>6440</v>
-      </c>
-      <c r="E5" t="n">
-        <v>3136</v>
-      </c>
-      <c r="F5" t="n">
-        <v>1508.5</v>
-      </c>
-      <c r="G5" t="n">
-        <v>1508.5</v>
-      </c>
-      <c r="H5" t="n">
-        <v>3136</v>
-      </c>
-      <c r="I5" t="n">
-        <v>1508.5</v>
-      </c>
-      <c r="J5" t="n">
-        <v>1508.5</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="B6" t="inlineStr">
+      <c r="A6" s="1" t="inlineStr">
         <is>
           <t>hesaplanan_asma</t>
         </is>
       </c>
+      <c r="B6" t="n">
+        <v>10</v>
+      </c>
       <c r="C6" t="n">
-        <v>10</v>
-      </c>
-      <c r="D6" t="n">
         <v>50</v>
-      </c>
-      <c r="E6" t="n">
-        <v>30</v>
-      </c>
-      <c r="F6" t="n">
-        <v>10</v>
-      </c>
-      <c r="G6" t="n">
-        <v>10</v>
-      </c>
-      <c r="H6" t="n">
-        <v>30</v>
-      </c>
-      <c r="I6" t="n">
-        <v>10</v>
-      </c>
-      <c r="J6" t="n">
-        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
a new property is imported in the part of the data visualization for creating graps in every minute
</commit_message>
<xml_diff>
--- a/kayitlarx.xlsx
+++ b/kayitlarx.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:J6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -435,79 +435,201 @@
   <sheetData>
     <row r="1">
       <c r="B1" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="n">
+      <c r="D1" s="1" t="n">
         <v>2</v>
+      </c>
+      <c r="E1" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="F1" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="G1" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="H1" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="I1" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="J1" s="1" t="n">
+        <v>8</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="1" t="inlineStr">
+      <c r="A2" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B2" t="inlineStr">
         <is>
           <t>carID</t>
         </is>
       </c>
-      <c r="B2" t="n">
+      <c r="C2" t="n">
         <v>1</v>
       </c>
-      <c r="C2" t="n">
+      <c r="D2" t="n">
         <v>2</v>
+      </c>
+      <c r="E2" t="n">
+        <v>3</v>
+      </c>
+      <c r="F2" t="n">
+        <v>4</v>
+      </c>
+      <c r="G2" t="n">
+        <v>6</v>
+      </c>
+      <c r="H2" t="n">
+        <v>9</v>
+      </c>
+      <c r="I2" t="n">
+        <v>12</v>
+      </c>
+      <c r="J2" t="n">
+        <v>12</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="1" t="inlineStr">
+      <c r="A3" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" t="inlineStr">
         <is>
           <t>speed2</t>
         </is>
       </c>
-      <c r="B3" t="n">
+      <c r="C3" t="n">
         <v>42.43</v>
       </c>
-      <c r="C3" t="n">
+      <c r="D3" t="n">
         <v>55.9</v>
+      </c>
+      <c r="E3" t="n">
+        <v>49.24</v>
+      </c>
+      <c r="F3" t="n">
+        <v>43.01</v>
+      </c>
+      <c r="G3" t="n">
+        <v>40.31</v>
+      </c>
+      <c r="H3" t="n">
+        <v>47.17</v>
+      </c>
+      <c r="I3" t="n">
+        <v>40.31</v>
+      </c>
+      <c r="J3" t="n">
+        <v>44.72</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="1" t="inlineStr">
+      <c r="A4" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="B4" t="inlineStr">
         <is>
           <t>asma</t>
         </is>
       </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>21.22</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>59.72</t>
-        </is>
+      <c r="C4" t="n">
+        <v>21.22</v>
+      </c>
+      <c r="D4" t="n">
+        <v>59.72</v>
+      </c>
+      <c r="E4" t="n">
+        <v>40.7</v>
+      </c>
+      <c r="F4" t="n">
+        <v>22.89</v>
+      </c>
+      <c r="G4" t="n">
+        <v>15.18</v>
+      </c>
+      <c r="H4" t="n">
+        <v>34.77</v>
+      </c>
+      <c r="I4" t="n">
+        <v>15.18</v>
+      </c>
+      <c r="J4" t="n">
+        <v>27.78</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="1" t="inlineStr">
+      <c r="A5" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="B5" t="inlineStr">
         <is>
           <t>ceza_tutar</t>
         </is>
       </c>
-      <c r="B5" t="n">
+      <c r="C5" t="n">
         <v>1508.5</v>
       </c>
-      <c r="C5" t="n">
+      <c r="D5" t="n">
         <v>6440</v>
+      </c>
+      <c r="E5" t="n">
+        <v>3136</v>
+      </c>
+      <c r="F5" t="n">
+        <v>1508.5</v>
+      </c>
+      <c r="G5" t="n">
+        <v>1508.5</v>
+      </c>
+      <c r="H5" t="n">
+        <v>3136</v>
+      </c>
+      <c r="I5" t="n">
+        <v>1508.5</v>
+      </c>
+      <c r="J5" t="n">
+        <v>1508.5</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="1" t="inlineStr">
+      <c r="A6" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="B6" t="inlineStr">
         <is>
           <t>hesaplanan_asma</t>
         </is>
       </c>
-      <c r="B6" t="n">
+      <c r="C6" t="n">
         <v>10</v>
       </c>
-      <c r="C6" t="n">
+      <c r="D6" t="n">
         <v>50</v>
+      </c>
+      <c r="E6" t="n">
+        <v>30</v>
+      </c>
+      <c r="F6" t="n">
+        <v>10</v>
+      </c>
+      <c r="G6" t="n">
+        <v>10</v>
+      </c>
+      <c r="H6" t="n">
+        <v>30</v>
+      </c>
+      <c r="I6" t="n">
+        <v>10</v>
+      </c>
+      <c r="J6" t="n">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
physical system is ready for sending data
</commit_message>
<xml_diff>
--- a/kayitlarx.xlsx
+++ b/kayitlarx.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:S6"/>
+  <dimension ref="A1:AH6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -488,6 +488,51 @@
       <c r="S1" s="1" t="n">
         <v>25</v>
       </c>
+      <c r="T1" s="1" t="n">
+        <v>27</v>
+      </c>
+      <c r="U1" s="1" t="n">
+        <v>28</v>
+      </c>
+      <c r="V1" s="1" t="n">
+        <v>29</v>
+      </c>
+      <c r="W1" s="1" t="n">
+        <v>30</v>
+      </c>
+      <c r="X1" s="1" t="n">
+        <v>34</v>
+      </c>
+      <c r="Y1" s="1" t="n">
+        <v>35</v>
+      </c>
+      <c r="Z1" s="1" t="n">
+        <v>36</v>
+      </c>
+      <c r="AA1" s="1" t="n">
+        <v>38</v>
+      </c>
+      <c r="AB1" s="1" t="n">
+        <v>39</v>
+      </c>
+      <c r="AC1" s="1" t="n">
+        <v>40</v>
+      </c>
+      <c r="AD1" s="1" t="n">
+        <v>41</v>
+      </c>
+      <c r="AE1" s="1" t="n">
+        <v>43</v>
+      </c>
+      <c r="AF1" s="1" t="n">
+        <v>42</v>
+      </c>
+      <c r="AG1" s="1" t="n">
+        <v>44</v>
+      </c>
+      <c r="AH1" s="1" t="n">
+        <v>45</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
@@ -549,6 +594,51 @@
       <c r="S2" t="n">
         <v>25</v>
       </c>
+      <c r="T2" t="n">
+        <v>27</v>
+      </c>
+      <c r="U2" t="n">
+        <v>28</v>
+      </c>
+      <c r="V2" t="n">
+        <v>30</v>
+      </c>
+      <c r="W2" t="n">
+        <v>30</v>
+      </c>
+      <c r="X2" t="n">
+        <v>34</v>
+      </c>
+      <c r="Y2" t="n">
+        <v>35</v>
+      </c>
+      <c r="Z2" t="n">
+        <v>36</v>
+      </c>
+      <c r="AA2" t="n">
+        <v>38</v>
+      </c>
+      <c r="AB2" t="n">
+        <v>39</v>
+      </c>
+      <c r="AC2" t="n">
+        <v>40</v>
+      </c>
+      <c r="AD2" t="n">
+        <v>43</v>
+      </c>
+      <c r="AE2" t="n">
+        <v>43</v>
+      </c>
+      <c r="AF2" t="n">
+        <v>43</v>
+      </c>
+      <c r="AG2" t="n">
+        <v>44</v>
+      </c>
+      <c r="AH2" t="n">
+        <v>45</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
@@ -610,6 +700,51 @@
       <c r="S3" t="n">
         <v>57.01</v>
       </c>
+      <c r="T3" t="n">
+        <v>50</v>
+      </c>
+      <c r="U3" t="n">
+        <v>80.62</v>
+      </c>
+      <c r="V3" t="n">
+        <v>42.72</v>
+      </c>
+      <c r="W3" t="n">
+        <v>75</v>
+      </c>
+      <c r="X3" t="n">
+        <v>40</v>
+      </c>
+      <c r="Y3" t="n">
+        <v>69.64</v>
+      </c>
+      <c r="Z3" t="n">
+        <v>80.62</v>
+      </c>
+      <c r="AA3" t="n">
+        <v>79.06</v>
+      </c>
+      <c r="AB3" t="n">
+        <v>47.43</v>
+      </c>
+      <c r="AC3" t="n">
+        <v>73.81999999999999</v>
+      </c>
+      <c r="AD3" t="n">
+        <v>63.64</v>
+      </c>
+      <c r="AE3" t="n">
+        <v>55.9</v>
+      </c>
+      <c r="AF3" t="n">
+        <v>55.9</v>
+      </c>
+      <c r="AG3" t="n">
+        <v>87.45999999999999</v>
+      </c>
+      <c r="AH3" t="n">
+        <v>69.45999999999999</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
@@ -707,6 +842,81 @@
           <t>62.88</t>
         </is>
       </c>
+      <c r="T4" t="inlineStr">
+        <is>
+          <t>42.86</t>
+        </is>
+      </c>
+      <c r="U4" t="inlineStr">
+        <is>
+          <t>130.35</t>
+        </is>
+      </c>
+      <c r="V4" t="inlineStr">
+        <is>
+          <t>22.06</t>
+        </is>
+      </c>
+      <c r="W4" t="inlineStr">
+        <is>
+          <t>114.29</t>
+        </is>
+      </c>
+      <c r="X4" t="inlineStr">
+        <is>
+          <t>14.29</t>
+        </is>
+      </c>
+      <c r="Y4" t="inlineStr">
+        <is>
+          <t>98.98</t>
+        </is>
+      </c>
+      <c r="Z4" t="inlineStr">
+        <is>
+          <t>130.35</t>
+        </is>
+      </c>
+      <c r="AA4" t="inlineStr">
+        <is>
+          <t>125.88</t>
+        </is>
+      </c>
+      <c r="AB4" t="inlineStr">
+        <is>
+          <t>35.53</t>
+        </is>
+      </c>
+      <c r="AC4" t="inlineStr">
+        <is>
+          <t>110.93</t>
+        </is>
+      </c>
+      <c r="AD4" t="inlineStr">
+        <is>
+          <t>81.83</t>
+        </is>
+      </c>
+      <c r="AE4" t="inlineStr">
+        <is>
+          <t>59.72</t>
+        </is>
+      </c>
+      <c r="AF4" t="inlineStr">
+        <is>
+          <t>59.72</t>
+        </is>
+      </c>
+      <c r="AG4" t="inlineStr">
+        <is>
+          <t>149.90</t>
+        </is>
+      </c>
+      <c r="AH4" t="inlineStr">
+        <is>
+          <t>98.46</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
@@ -768,6 +978,51 @@
       <c r="S5" t="n">
         <v>6440</v>
       </c>
+      <c r="T5" t="n">
+        <v>3136</v>
+      </c>
+      <c r="U5" t="n">
+        <v>6440</v>
+      </c>
+      <c r="V5" t="n">
+        <v>1508.5</v>
+      </c>
+      <c r="W5" t="n">
+        <v>6440</v>
+      </c>
+      <c r="X5" t="n">
+        <v>1508.5</v>
+      </c>
+      <c r="Y5" t="n">
+        <v>6440</v>
+      </c>
+      <c r="Z5" t="n">
+        <v>6440</v>
+      </c>
+      <c r="AA5" t="n">
+        <v>6440</v>
+      </c>
+      <c r="AB5" t="n">
+        <v>3136</v>
+      </c>
+      <c r="AC5" t="n">
+        <v>6440</v>
+      </c>
+      <c r="AD5" t="n">
+        <v>6440</v>
+      </c>
+      <c r="AE5" t="n">
+        <v>6440</v>
+      </c>
+      <c r="AF5" t="n">
+        <v>6440</v>
+      </c>
+      <c r="AG5" t="n">
+        <v>6440</v>
+      </c>
+      <c r="AH5" t="n">
+        <v>6440</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="inlineStr">
@@ -827,6 +1082,51 @@
         <v>50</v>
       </c>
       <c r="S6" t="n">
+        <v>50</v>
+      </c>
+      <c r="T6" t="n">
+        <v>30</v>
+      </c>
+      <c r="U6" t="n">
+        <v>50</v>
+      </c>
+      <c r="V6" t="n">
+        <v>10</v>
+      </c>
+      <c r="W6" t="n">
+        <v>50</v>
+      </c>
+      <c r="X6" t="n">
+        <v>10</v>
+      </c>
+      <c r="Y6" t="n">
+        <v>50</v>
+      </c>
+      <c r="Z6" t="n">
+        <v>50</v>
+      </c>
+      <c r="AA6" t="n">
+        <v>50</v>
+      </c>
+      <c r="AB6" t="n">
+        <v>30</v>
+      </c>
+      <c r="AC6" t="n">
+        <v>50</v>
+      </c>
+      <c r="AD6" t="n">
+        <v>50</v>
+      </c>
+      <c r="AE6" t="n">
+        <v>50</v>
+      </c>
+      <c r="AF6" t="n">
+        <v>50</v>
+      </c>
+      <c r="AG6" t="n">
+        <v>50</v>
+      </c>
+      <c r="AH6" t="n">
         <v>50</v>
       </c>
     </row>

</xml_diff>